<commit_message>
ADC branch of psoc and calibration files
</commit_message>
<xml_diff>
--- a/calibration_data_20180815.xlsx
+++ b/calibration_data_20180815.xlsx
@@ -5,27 +5,33 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\OneDrive\Engineering\2018\TRC4000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\Hydraulic-Mimic-Arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1EEFE56A-E0E7-4F43-907E-6C9E48658509}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{52B5FA82-BEF9-4A09-B24A-1711BF4BF7D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F94D97-9CFA-429A-A80F-778055E19EC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9420" xr2:uid="{5962F5FD-9C27-4C35-8D6C-2DFABD9CE811}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9420" activeTab="1" xr2:uid="{5962F5FD-9C27-4C35-8D6C-2DFABD9CE811}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Proximal to Metacarpal angle</t>
   </si>
@@ -37,6 +43,18 @@
   </si>
   <si>
     <t>Pot1 (/4095)</t>
+  </si>
+  <si>
+    <t>Mid-Prox</t>
+  </si>
+  <si>
+    <t>Palm-Prox</t>
+  </si>
+  <si>
+    <t>Prox ADC</t>
+  </si>
+  <si>
+    <t>Mid ADC</t>
   </si>
 </sst>
 </file>
@@ -408,7 +426,828 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prox ADC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>185.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>171.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1593</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1414</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F645-44B1-B736-54C943188C24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="432315760"/>
+        <c:axId val="435984056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="432315760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435984056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435984056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="432315760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.2684698162729659"/>
+                  <c:y val="-0.29795968212306795"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$15:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>193.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$15:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.300000000000011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14CD-4DE6-8A35-2ADD2B7869B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="440801240"/>
+        <c:axId val="440802880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="440801240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440802880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="440802880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440801240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -964,6 +1803,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -997,6 +2868,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD51F8F1-8D3D-4AD7-8AC7-797C0A2B1ADE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD553381-F4C1-4694-A4C6-29E2DFAFAF87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1304,7 +3252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C3A3C3-A19B-4696-9FE0-B53E26D2DA7E}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="D1" activeCellId="1" sqref="A1:A11 D1:D11"/>
     </sheetView>
   </sheetViews>
@@ -1474,4 +3422,312 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4FA85F-AB27-4F99-81D5-8E159AB5FDC7}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" activeCellId="1" sqref="A15:A21 E15:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>185.5</v>
+      </c>
+      <c r="B2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>171.4</v>
+      </c>
+      <c r="B3">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>159.1</v>
+      </c>
+      <c r="B4">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="B5">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>125.4</v>
+      </c>
+      <c r="B6">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>107.2</v>
+      </c>
+      <c r="B7">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>192.2</v>
+      </c>
+      <c r="B8">
+        <v>1890</v>
+      </c>
+      <c r="C8">
+        <v>176.7</v>
+      </c>
+      <c r="D8">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>192.2</v>
+      </c>
+      <c r="B9">
+        <v>1890</v>
+      </c>
+      <c r="C9">
+        <v>166.4</v>
+      </c>
+      <c r="D9">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>192.2</v>
+      </c>
+      <c r="B10">
+        <v>1890</v>
+      </c>
+      <c r="C10">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="D10">
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>192.2</v>
+      </c>
+      <c r="B11">
+        <v>1890</v>
+      </c>
+      <c r="C11">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="D11">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>192.2</v>
+      </c>
+      <c r="B12">
+        <v>1890</v>
+      </c>
+      <c r="C12">
+        <v>125.6</v>
+      </c>
+      <c r="D12">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>192.2</v>
+      </c>
+      <c r="B13">
+        <v>1890</v>
+      </c>
+      <c r="C13">
+        <v>112.6</v>
+      </c>
+      <c r="D13">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>192.2</v>
+      </c>
+      <c r="B14">
+        <v>1890</v>
+      </c>
+      <c r="C14">
+        <v>101.1</v>
+      </c>
+      <c r="D14">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>193.3</v>
+      </c>
+      <c r="B15">
+        <v>1891</v>
+      </c>
+      <c r="C15">
+        <v>101.1</v>
+      </c>
+      <c r="D15">
+        <v>2244</v>
+      </c>
+      <c r="E15">
+        <f>C15-$C$14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>180</v>
+      </c>
+      <c r="B16">
+        <v>1777</v>
+      </c>
+      <c r="C16">
+        <v>104</v>
+      </c>
+      <c r="D16">
+        <v>2244</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E21" si="0">C16-$C$14</f>
+        <v>2.9000000000000057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="B17">
+        <v>1620</v>
+      </c>
+      <c r="C17">
+        <v>118.7</v>
+      </c>
+      <c r="D17">
+        <v>2244</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>17.600000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>154</v>
+      </c>
+      <c r="B18">
+        <v>1534</v>
+      </c>
+      <c r="C18">
+        <v>127.1</v>
+      </c>
+      <c r="D18">
+        <v>2244</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="B19">
+        <v>1358</v>
+      </c>
+      <c r="C19">
+        <v>140.9</v>
+      </c>
+      <c r="D19">
+        <v>2244</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>39.800000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>113.1</v>
+      </c>
+      <c r="B20">
+        <v>1192</v>
+      </c>
+      <c r="C20">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="D20">
+        <v>2244</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>49.099999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>103.2</v>
+      </c>
+      <c r="B21">
+        <v>1157</v>
+      </c>
+      <c r="C21">
+        <v>154.4</v>
+      </c>
+      <c r="D21">
+        <v>2244</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>53.300000000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>